<commit_message>
FInished implementing excel calendar.
</commit_message>
<xml_diff>
--- a/sampleData.export.xlsx
+++ b/sampleData.export.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -405,145 +405,122 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>26/-1</v>
+        <v>27/11</v>
       </c>
       <c r="B2" t="str">
-        <v>27/-1</v>
+        <v>28/11</v>
       </c>
       <c r="C2" t="str">
-        <v>28/-1</v>
+        <v>29/11</v>
       </c>
       <c r="D2" t="str">
-        <v>29/-1</v>
+        <v>30/11</v>
       </c>
       <c r="E2" t="str">
-        <v>30/-1</v>
+        <v>1/12</v>
       </c>
       <c r="F2" t="str">
-        <v>31/-1</v>
+        <v>2/12</v>
       </c>
       <c r="G2" t="str">
-        <v>1/0</v>
+        <v>3/12</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>2/0</v>
+        <v>4/12</v>
       </c>
       <c r="B3" t="str">
-        <v>3/0</v>
+        <v>5/12</v>
       </c>
       <c r="C3" t="str">
-        <v>4/0</v>
+        <v>6/12</v>
       </c>
       <c r="D3" t="str">
-        <v>5/0</v>
+        <v>7/12</v>
       </c>
       <c r="E3" t="str">
-        <v>6/0</v>
+        <v>8/12</v>
       </c>
       <c r="F3" t="str">
-        <v>7/0</v>
+        <v>9/12</v>
       </c>
       <c r="G3" t="str">
-        <v>8/0</v>
+        <v>10/12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>9/0</v>
+        <v>11/12</v>
       </c>
       <c r="B4" t="str">
-        <v>10/0</v>
+        <v>12/12</v>
       </c>
       <c r="C4" t="str">
-        <v>11/0</v>
+        <v>13/12</v>
       </c>
       <c r="D4" t="str">
-        <v>12/0</v>
+        <v>14/12</v>
       </c>
       <c r="E4" t="str">
-        <v>13/0</v>
+        <v>15/12</v>
       </c>
       <c r="F4" t="str">
-        <v>14/0</v>
+        <v>16/12</v>
       </c>
       <c r="G4" t="str">
-        <v>15/0</v>
+        <v>17/12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>16/0</v>
+        <v>18/12</v>
       </c>
       <c r="B5" t="str">
-        <v>17/0</v>
+        <v>19/12</v>
       </c>
       <c r="C5" t="str">
-        <v>18/0</v>
+        <v>20/12</v>
       </c>
       <c r="D5" t="str">
-        <v>19/0</v>
+        <v>21/12</v>
       </c>
       <c r="E5" t="str">
-        <v>20/0</v>
+        <v>22/12</v>
       </c>
       <c r="F5" t="str">
-        <v>21/0</v>
+        <v>23/12</v>
       </c>
       <c r="G5" t="str">
-        <v>22/0</v>
+        <v>24/12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>23/0</v>
+        <v>25/12</v>
       </c>
       <c r="B6" t="str">
-        <v>24/0</v>
+        <v>26/12</v>
       </c>
       <c r="C6" t="str">
-        <v>25/0</v>
+        <v>27/12</v>
       </c>
       <c r="D6" t="str">
-        <v>26/0</v>
+        <v>28/12</v>
       </c>
       <c r="E6" t="str">
-        <v>27/0</v>
+        <v>29/12</v>
       </c>
       <c r="F6" t="str">
-        <v>28/0</v>
+        <v>30/12</v>
       </c>
       <c r="G6" t="str">
-        <v>29/0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>30/0</v>
-      </c>
-      <c r="B7" t="str">
-        <v>31/0</v>
-      </c>
-      <c r="C7" t="str">
-        <v>1/1</v>
-      </c>
-      <c r="D7" t="str">
-        <v>2/1</v>
-      </c>
-      <c r="E7" t="str">
-        <v>3/1</v>
-      </c>
-      <c r="F7" t="str">
-        <v>4/1</v>
-      </c>
-      <c r="G7" t="str">
-        <v>5/1</v>
+        <v>31/12</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>